<commit_message>
Everything up to date
</commit_message>
<xml_diff>
--- a/doc/Case List.xlsx
+++ b/doc/Case List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Case List</t>
   </si>
@@ -73,19 +73,107 @@
   </si>
   <si>
     <t>Conversion Bays</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>NZXT</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>Crafted</t>
+  </si>
+  <si>
+    <t>http://www.nzxt.com/new/products/crafted_series/phantom</t>
+  </si>
+  <si>
+    <t>http://www.google.com/search?sourceid=chrome&amp;ie=UTF-8&amp;q=NZXT+Phantom#q=NZXT+Phantom&amp;um=1&amp;ie=UTF-8&amp;tbo=u&amp;tbs=shop:1&amp;fp=1</t>
+  </si>
+  <si>
+    <t>Full Tower</t>
+  </si>
+  <si>
+    <t>MaxCoolerHeight</t>
+  </si>
+  <si>
+    <t>MaxGpuLength</t>
+  </si>
+  <si>
+    <t>EATX/ATX/Micro ATX</t>
+  </si>
+  <si>
+    <t>Vulcan</t>
+  </si>
+  <si>
+    <t>http://www.nzxt.com/new/products/crafted_series/vulcan</t>
+  </si>
+  <si>
+    <t>http://www.google.com/products/catalog?hl=en&amp;safe=off&amp;q=NZXT+Vulcan&amp;um=1&amp;ie=UTF-8&amp;cid=18143607670069501874#</t>
+  </si>
+  <si>
+    <t>Mini Tower</t>
+  </si>
+  <si>
+    <t>Micro ATX</t>
+  </si>
+  <si>
+    <t>RC-342-KKN2-GP</t>
+  </si>
+  <si>
+    <t>Cooler Master</t>
+  </si>
+  <si>
+    <t>http://www.coolermaster-usa.com/product.php?category_id=20&amp;product_id=2962</t>
+  </si>
+  <si>
+    <t>http://www.google.com/search?q=RC-342-KKN2-GP&amp;hl=en&amp;tbs=shop:1&amp;aq=f</t>
+  </si>
+  <si>
+    <t>http://www.google.com/search?sourceid=chrome&amp;ie=UTF-8&amp;q=NV-942-KKN1#q=NV-942-KKN1&amp;um=1&amp;ie=UTF-8&amp;tbo=u&amp;tbs=shop:1&amp;fp=1</t>
+  </si>
+  <si>
+    <t>http://www.coolermaster-usa.com/product.php?category_id=18&amp;product_id=3017</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>NV-942-KKN1</t>
+  </si>
+  <si>
+    <t>HAF</t>
+  </si>
+  <si>
+    <t>XL ATX/EATX/ATX/Micro ATX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,16 +193,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -430,16 +525,18 @@
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -492,14 +589,279 @@
         <v>14</v>
       </c>
       <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4">
+        <v>623</v>
+      </c>
+      <c r="P4">
+        <v>222</v>
+      </c>
+      <c r="Q4">
+        <v>540</v>
+      </c>
+      <c r="R4">
+        <v>165</v>
+      </c>
+      <c r="S4">
+        <v>350</v>
+      </c>
+      <c r="T4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>406</v>
+      </c>
+      <c r="P5">
+        <v>180</v>
+      </c>
+      <c r="Q5">
+        <v>422</v>
+      </c>
+      <c r="R5">
+        <v>165</v>
+      </c>
+      <c r="S5">
+        <v>350</v>
+      </c>
+      <c r="T5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6">
+        <v>440</v>
+      </c>
+      <c r="P6">
+        <v>180</v>
+      </c>
+      <c r="Q6">
+        <v>353</v>
+      </c>
+      <c r="R6">
+        <v>140</v>
+      </c>
+      <c r="S6">
+        <v>245</v>
+      </c>
+      <c r="T6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>230</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <v>550</v>
+      </c>
+      <c r="P7">
+        <v>230</v>
+      </c>
+      <c r="Q7">
+        <v>590</v>
+      </c>
+      <c r="R7">
+        <v>170</v>
+      </c>
+      <c r="S7">
+        <v>350</v>
+      </c>
+      <c r="T7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2" location="q=NZXT+Phantom&amp;um=1&amp;ie=UTF-8&amp;tbo=u&amp;tbs=shop:1&amp;fp=1" display="http://www.google.com/search?sourceid=chrome&amp;ie=UTF-8&amp;q=NZXT+Phantom - q=NZXT+Phantom&amp;um=1&amp;ie=UTF-8&amp;tbo=u&amp;tbs=shop:1&amp;fp=1"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4" display="http://www.google.com/products/catalog?hl=en&amp;safe=off&amp;q=NZXT+Vulcan&amp;um=1&amp;ie=UTF-8&amp;cid=18143607670069501874"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7" location="q=NV-942-KKN1&amp;um=1&amp;ie=UTF-8&amp;tbo=u&amp;tbs=shop:1&amp;fp=1" display="http://www.google.com/search?sourceid=chrome&amp;ie=UTF-8&amp;q=NV-942-KKN1 - q=NV-942-KKN1&amp;um=1&amp;ie=UTF-8&amp;tbo=u&amp;tbs=shop:1&amp;fp=1"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>